<commit_message>
data for new shooter wheel calibration
</commit_message>
<xml_diff>
--- a/shooter_data.xlsx
+++ b/shooter_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="14355" windowHeight="4935"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="14355" windowHeight="4935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,18 +16,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>POWER</t>
   </si>
   <si>
     <t>AVG_RPM</t>
   </si>
+  <si>
+    <t>Friday 3/22 Evening</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -57,9 +63,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -221,11 +228,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="6163072"/>
-        <c:axId val="6161536"/>
+        <c:axId val="75822592"/>
+        <c:axId val="75824128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="6163072"/>
+        <c:axId val="75822592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -235,12 +242,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="6161536"/>
+        <c:crossAx val="75824128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="6161536"/>
+        <c:axId val="75824128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -251,7 +258,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="6163072"/>
+        <c:crossAx val="75822592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -386,11 +393,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="98606464"/>
-        <c:axId val="98604928"/>
+        <c:axId val="76517376"/>
+        <c:axId val="76518912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98606464"/>
+        <c:axId val="76517376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -400,12 +407,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98604928"/>
+        <c:crossAx val="76518912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98604928"/>
+        <c:axId val="76518912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -416,7 +423,384 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98606464"/>
+        <c:crossAx val="76517376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>AvgRpm-Power</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$4:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$4:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>759.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1095.0999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1352.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1579.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1777.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1982.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2210.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2391.6999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2594.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2765</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2890.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3067.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3233.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3426.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3583</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3812.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="54600832"/>
+        <c:axId val="54594944"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="54600832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="54594944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="54594944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="54600832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>mid range</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="#,##0.000000000000" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$9:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1982.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2210.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2391.6999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2594.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2765</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2890.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3067.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$9:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="54554624"/>
+        <c:axId val="53852416"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="54554624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="53852416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="53852416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="54554624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -482,6 +866,71 @@
       <xdr:colOff>371474</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -792,7 +1241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -936,13 +1385,158 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="B4" s="2">
+        <v>759.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1095.0999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1352.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1579.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1777.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1982.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2210.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2391.6999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2594.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2765</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2890.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="B15" s="2">
+        <v>3067.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="B16" s="2">
+        <v>3233.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B17" s="2">
+        <v>3426.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="B18" s="2">
+        <v>3583</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2">
+        <v>3812.6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>